<commit_message>
corrigindo uso do termo plataforma no PB
</commit_message>
<xml_diff>
--- a/Documentos-projeto-gofreela/PB-goFreela.xlsx
+++ b/Documentos-projeto-gofreela/PB-goFreela.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/13923b2f950de320/UNIPE_SPI_4_ANA/PROJ_INTERDISCIPLINAR/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/13923b2f950de320/UNIPE_SPI_4_ANA/PROJ_INTERDISCIPLINAR/PB/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="520" documentId="13_ncr:1_{738E3B96-06C4-4B4F-BA6C-5B9750DE4F5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E563E80A-0BC6-417C-B720-A05D9A70DCBA}"/>
+  <xr:revisionPtr revIDLastSave="542" documentId="13_ncr:1_{738E3B96-06C4-4B4F-BA6C-5B9750DE4F5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A0A34D67-E29C-46B0-ABF4-2E270925527C}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -256,26 +256,29 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Cadastro de Empresas</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">: As empresas contratantes </t>
+    <t>Essencial</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Troca ou Recuperação de Senha:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> O sistema </t>
     </r>
     <r>
       <rPr>
@@ -286,62 +289,40 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>devem</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>poder</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> se cadastrar na plataforma, fornecendo informações detalhadas sobre a empresa, incluindo nome, localização, área de atuação e contato.</t>
-    </r>
-  </si>
-  <si>
-    <t>Essencial</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Cadastro de Profissionais Autônomos</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">: Os profissionais autônomos </t>
+      <t>deve</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> permitir a opção de alteração e recuperação de senhas de usuários cadastrados.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Autenticação de usuários:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> O sistema </t>
     </r>
     <r>
       <rPr>
@@ -352,50 +333,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>devem</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> poder se cadastrar na plataforma, criando perfis individuais com informações sobre suas habilidades, experiência, portfólio, e outras informações relevantes para os potenciais empregadores.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Troca ou Recuperação de Senha:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> O sistema </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>deve</t>
     </r>
     <r>
@@ -406,95 +343,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> permitir a opção de alteração e recuperação de senhas de usuários cadastrados.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Autenticação de usuários:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> O sistema </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>deve</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t xml:space="preserve"> permitir autenticar cadastro de usuários com envio de e-mail de boas vindas com senha provisória e link de autenticação.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Login de usuários:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> O sistema </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>deve</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> permitir aos usuários cadastrados poder fazer login na plataforma usando suas credenciais para ter acesso às funcionalidades do sistema.</t>
     </r>
   </si>
   <si>
@@ -528,117 +377,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>US-ID 1:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Como uma empresa contratante, eu quero poder me cadastrar na plataforma GoFreela para fornecer informações detalhadas sobre minha empresa, incluindo nome, localização, área de atuação e contato, para que eu possa publicar projetos e atrair profissionais autônomos qualificados.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">US-ID 2: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Como um profissional autônomo, eu quero criar um perfil individual na plataforma GoFreela com informações sobre minhas habilidades, experiência, portfólio e outras informações relevantes para potenciais empregadores, para que eu possa me candidatar a projetos e ser contratado.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>US-ID 3</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">: Como Contratante e Profissional Autônomo, eu quero receber um e-mail de boas-vindas com uma senha provisória e um link de autenticação após o cadastro, para que eu possa confirmar minha conta e acessar a plataforma.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>US-ID 4:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Como um usuário registrado (Contratante,  Profissional Autônomo e analista de suporte técnico), eu quero fazer login na plataforma GoFreela usando minhas credenciais, para acessar as funcionalidades da plataforma.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>US-ID 5</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: Como Contratante e Profissional Autônomo, eu quero ter a opção de trocar ou recuperar minha senha, caso eu a esqueça ou deseje alterá-la.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>Publicação de Projetos</t>
     </r>
     <r>
@@ -718,184 +456,7 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Painel Personalizado para Empresas:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Cada empresa </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>deve</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> ter um painel personalizado que exiba informações sobre projetos publicados, candidatos selecionados, projetos em andamento e avaliações recebidas.</t>
-    </r>
-  </si>
-  <si>
     <t>Importante</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Painel Personalizado para Profissionais:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Cada profissional autônomo </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>deve</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> ter um painel personalizado que mostre projetos aplicados, projetos em andamento, mensagens recebidas, avaliações recebidas e outras atividades relacionadas ao seu trabalho na plataforma.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>US-ID 1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">: Como contratante, eu quero poder publicar detalhes sobre os projetos que desejo contratar na plataforma GoFreela, incluindo descrição do projeto, habilidades necessárias, prazo de entrega, orçamento disponível e link orientado para contato direto, para atrair profissionais adequados.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>US-ID 2:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Como um profissional autônomo, eu quero poder pesquisar e filtrar projetos na plataforma GoFreela com base em habilidades, área de interesse, localização e outros critérios relevantes, para encontrar projetos adequados.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>US-ID 3:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Como uma empresa contratante, eu quero ter um painel personalizado na plataforma GoFreela que exiba informações sobre projetos publicados, candidatos selecionados, projetos em andamento e avaliações recebidas, para gerenciar eficientemente as contratações.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>US-ID 4:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Como um profissional autônomo, eu quero ter um painel personalizado na plataforma GoFreela que mostre projetos aplicados, projetos em andamento, mensagens recebidas, avaliações recebidas e outras atividades relacionadas ao meu trabalho na plataforma, para facilitar o acompanhamento das oportunidades.</t>
-    </r>
   </si>
   <si>
     <t>1
@@ -1004,164 +565,7 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Suporte ao Cliente:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> O sistema </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>deve</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> permitir ao  analista de suporte ao cliente: fornecer assistência aos usuários, solucionar problemas técnicos, esclarecer dúvidas e auxiliar tanto empresas quanto profissionais autônomos durante o uso da plataforma.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Gamificação:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Implementar um sistema de gamificação onde os usuários acumulam pontos, distintivos ou outros tipos de reconhecimento com base em seu desempenho, avaliações positivas e participação ativa na plataforma. Isso pode aumentar o engajamento e incentivar a qualidade nos serviços prestados.</t>
-    </r>
-  </si>
-  <si>
     <t>Desejável</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>US-ID 1:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Como um profissional autônomo, eu quero me candidatar a projetos na plataforma GoFreela, enviando propostas e informações adicionais para as empresas contratantes, para ser considerado para o projeto.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>US-ID 2:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Como uma empresa contratante, eu quero poder avaliar o desempenho dos profissionais autônomos após a conclusão do projeto, incluindo feedback detalhado sobre o trabalho realizado, qualidade, cumprimento de prazos e outras métricas relevantes, para garantir uma experiência de contratação transparente.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-US-ID 3:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Como Contratante e Profissional Autônomo da plataforma GoFreela, eu quero ter acesso a um analista de suporte ao cliente que pode fornecer assistência, solucionar problemas técnicos e esclarecer dúvidas, para garantir uma experiência positiva na plataforma.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>US-ID 4</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: Como um usuário da plataforma GoFreela, eu quero acumular pontos e distintivos com base no meu desempenho, avaliações positivas e participação ativa na plataforma, para aumentar meu engajamento e reconhecimento na comunidade de freelancers.</t>
-    </r>
   </si>
   <si>
     <t>US-ID1 - Essencial
@@ -1219,13 +623,656 @@
   </si>
   <si>
     <t>O sistema deve ser modular e ter um código bem estruturado para facilitar atualizações, correções de bugs e incorporação de novos recursos no futuro.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Painel Personalizado para Empresas:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Cada empresa </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>deve</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ter um painel personalizado que exiba informações sobre projetos publicados, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>candidatos selecionados,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>projetos em andamento</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> e</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> avaliações recebidas.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Cadastro de Empresas</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: As empresas contratantes </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>devem</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>poder</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> se cadastrar no sistema, fornecendo informações detalhadas sobre a empresa, incluindo nome, localização, área de atuação e contato.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Cadastro de Profissionais Autônomos</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: Os profissionais autônomos </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>devem</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> poder se cadastrar no sistema, criando perfis individuais com informações sobre suas habilidades, experiência, portfólio, e outras informações relevantes para os potenciais empregadores.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Login de usuários:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> O sistema </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>deve</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> permitir aos usuários cadastrados poder fazer login no sistema usando suas credenciais para ter acesso às funcionalidades do sistema.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Suporte ao Cliente:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> O sistema </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>deve</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> permitir ao  analista de suporte ao cliente: fornecer assistência aos usuários, solucionar problemas técnicos, esclarecer dúvidas e auxiliar tanto empresas quanto profissionais autônomos durante o uso do sistema.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>US-ID 1:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Como um profissional autônomo, eu quero me candidatar a projetos no sistema GoFreela, enviando propostas e informações adicionais para as empresas contratantes, para ser considerado para o projeto.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>US-ID 2:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Como uma empresa contratante, eu quero poder avaliar o desempenho dos profissionais autônomos após a conclusão do projeto, incluindo feedback detalhado sobre o trabalho realizado, qualidade, cumprimento de prazos e outras métricas relevantes, para garantir uma experiência de contratação transparente.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+US-ID 3:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Como Contratante e Profissional Autônomo do sistema GoFreela, eu quero ter acesso a um analista de suporte ao cliente que pode fornecer assistência, solucionar problemas técnicos e esclarecer dúvidas, para garantir uma experiência positiva no sistema.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>US-ID 4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Como um usuário do GoFreela, eu quero acumular pontos e distintivos com base no meu desempenho, avaliações positivas e participação ativa no sisistema, para aumentar meu engajamento e reconhecimento na comunidade de freelancers.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>US-ID 1:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Como uma empresa contratante, eu quero poder me cadastrar no sistema GoFreela para fornecer informações detalhadas sobre minha empresa, incluindo nome, localização, área de atuação e contato, para que eu possa publicar projetos e atrair profissionais autônomos qualificados.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">US-ID 2: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Como um profissional autônomo, eu quero criar um perfil individual no sistema GoFreela com informações sobre minhas habilidades, experiência, portfólio e outras informações relevantes para potenciais empregadores, para que eu possa me candidatar a projetos e ser contratado.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>US-ID 3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: Como Contratante e Profissional Autônomo, eu quero receber um e-mail de boas-vindas com uma senha provisória e um link de autenticação após o cadastro, para que eu possa confirmar minha conta e acessar o sistema.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>US-ID 4:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Como um usuário registrado (Contratante,  Profissional Autônomo e analista de suporte técnico), eu quero fazer login no sistema GoFreela usando minhas credenciais, para acessar as funcionalidades do sistema.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>US-ID 5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Como Contratante e Profissional Autônomo, eu quero ter a opção de trocar ou recuperar minha senha, caso eu a esqueça ou deseje alterá-la.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>US-ID 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: Como contratante, eu quero poder publicar detalhes sobre os projetos que desejo contratar no sistema GoFreela, incluindo descrição do projeto, habilidades necessárias, prazo de entrega, orçamento disponível e link orientado para contato direto, para atrair profissionais adequados.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>US-ID 2:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Como um profissional autônomo, eu quero poder pesquisar e filtrar projetos no sistema GoFreela com base em habilidades, área de interesse, localização e outros critérios relevantes, para encontrar projetos adequados.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>US-ID 3:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Como uma empresa contratante, eu quero ter um painel personalizado no sistema GoFreela que exiba informações sobre projetos publicados, candidatos selecionados, projetos em andamento e avaliações recebidas, para gerenciar eficientemente as contratações.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>US-ID 4:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Como um profissional autônomo, eu quero ter um painel personalizado no sistema GoFreela que mostre projetos aplicados, projetos em andamento, mensagens recebidas, avaliações recebidas e outras atividades relacionadas ao meu trabalho no sistema, para facilitar o acompanhamento das oportunidades.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Gamificação:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Implementar um sistema de gamificação onde os usuários acumulam pontos, distintivos ou outros tipos de reconhecimento com base em seu desempenho, avaliações positivas e participação ativa no site. Isso pode aumentar o engajamento e incentivar a qualidade nos serviços prestados.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Painel Personalizado para Profissionais:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Cada profissional autônomo </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>deve</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ter um painel personalizado que mostre projetos aplicados, projetos em andamento, mensagens recebidas, avaliações recebidas e outras atividades relacionadas ao seu trabalho no sistema.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1404,6 +1451,13 @@
       <b/>
       <sz val="12"/>
       <color rgb="FF002060"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF7030A0"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1735,7 +1789,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1815,6 +1869,27 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1828,14 +1903,83 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1843,102 +1987,11 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1954,10 +2007,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2164,8 +2213,8 @@
   </sheetPr>
   <dimension ref="A1:HC8"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="83" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView topLeftCell="A7" zoomScale="83" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2179,36 +2228,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:211" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="33"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="40"/>
     </row>
     <row r="2" spans="1:211" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="34"/>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="36"/>
+      <c r="A2" s="41"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="43"/>
     </row>
     <row r="3" spans="1:211" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="37"/>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="39"/>
+      <c r="A3" s="44"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="46"/>
     </row>
     <row r="4" spans="1:211" s="4" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="64" t="s">
+      <c r="A4" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="65"/>
-      <c r="C4" s="65"/>
-      <c r="D4" s="65"/>
-      <c r="E4" s="66"/>
+      <c r="B4" s="48"/>
+      <c r="C4" s="48"/>
+      <c r="D4" s="48"/>
+      <c r="E4" s="49"/>
       <c r="F4"/>
       <c r="G4"/>
       <c r="H4"/>
@@ -2647,13 +2696,13 @@
         <v>26</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E6" s="63" t="s">
-        <v>36</v>
+        <v>68</v>
+      </c>
+      <c r="E6" s="32" t="s">
+        <v>33</v>
       </c>
       <c r="F6"/>
       <c r="G6"/>
@@ -2867,16 +2916,16 @@
         <v>2</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E7" s="63" t="s">
-        <v>48</v>
+        <v>69</v>
+      </c>
+      <c r="E7" s="32" t="s">
+        <v>41</v>
       </c>
       <c r="F7"/>
       <c r="G7"/>
@@ -3090,16 +3139,16 @@
         <v>3</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E8" s="63" t="s">
-        <v>54</v>
+        <v>67</v>
+      </c>
+      <c r="E8" s="32" t="s">
+        <v>44</v>
       </c>
       <c r="F8"/>
       <c r="G8"/>
@@ -3326,8 +3375,8 @@
   </sheetPr>
   <dimension ref="A1:AJ21"/>
   <sheetViews>
-    <sheetView zoomScale="114" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+    <sheetView topLeftCell="A13" zoomScale="114" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3340,34 +3389,33 @@
     <col min="7" max="7" width="10.28515625" customWidth="1"/>
     <col min="8" max="8" width="9.42578125" customWidth="1"/>
     <col min="9" max="9" width="58.28515625" customWidth="1"/>
-    <col min="10" max="36" width="12.7109375" style="62"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="15"/>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="68" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
     </row>
     <row r="2" spans="1:36" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="71" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="69"/>
+      <c r="B2" s="71"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="71"/>
+      <c r="I2" s="72"/>
     </row>
     <row r="3" spans="1:36" s="4" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="16"/>
@@ -3391,77 +3439,77 @@
       </c>
       <c r="H3" s="54"/>
       <c r="I3" s="55"/>
-      <c r="J3" s="62"/>
-      <c r="K3" s="62"/>
-      <c r="L3" s="62"/>
-      <c r="M3" s="62"/>
-      <c r="N3" s="62"/>
-      <c r="O3" s="62"/>
-      <c r="P3" s="62"/>
-      <c r="Q3" s="62"/>
-      <c r="R3" s="62"/>
-      <c r="S3" s="62"/>
-      <c r="T3" s="62"/>
-      <c r="U3" s="62"/>
-      <c r="V3" s="62"/>
-      <c r="W3" s="62"/>
-      <c r="X3" s="62"/>
-      <c r="Y3" s="62"/>
-      <c r="Z3" s="62"/>
-      <c r="AA3" s="62"/>
-      <c r="AB3" s="62"/>
-      <c r="AC3" s="62"/>
-      <c r="AD3" s="62"/>
-      <c r="AE3" s="62"/>
-      <c r="AF3" s="62"/>
-      <c r="AG3" s="62"/>
-      <c r="AH3" s="62"/>
-      <c r="AI3" s="62"/>
-      <c r="AJ3" s="62"/>
+      <c r="J3"/>
+      <c r="K3"/>
+      <c r="L3"/>
+      <c r="M3"/>
+      <c r="N3"/>
+      <c r="O3"/>
+      <c r="P3"/>
+      <c r="Q3"/>
+      <c r="R3"/>
+      <c r="S3"/>
+      <c r="T3"/>
+      <c r="U3"/>
+      <c r="V3"/>
+      <c r="W3"/>
+      <c r="X3"/>
+      <c r="Y3"/>
+      <c r="Z3"/>
+      <c r="AA3"/>
+      <c r="AB3"/>
+      <c r="AC3"/>
+      <c r="AD3"/>
+      <c r="AE3"/>
+      <c r="AF3"/>
+      <c r="AG3"/>
+      <c r="AH3"/>
+      <c r="AI3"/>
+      <c r="AJ3"/>
     </row>
     <row r="4" spans="1:36" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="47" t="s">
+      <c r="B4" s="69" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="48"/>
-      <c r="D4" s="45" t="s">
+      <c r="C4" s="70"/>
+      <c r="D4" s="60" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="46"/>
+      <c r="E4" s="61"/>
       <c r="F4" s="21"/>
-      <c r="G4" s="56"/>
-      <c r="H4" s="57"/>
-      <c r="I4" s="58"/>
-      <c r="J4" s="62"/>
-      <c r="K4" s="62"/>
-      <c r="L4" s="62"/>
-      <c r="M4" s="62"/>
-      <c r="N4" s="62"/>
-      <c r="O4" s="62"/>
-      <c r="P4" s="62"/>
-      <c r="Q4" s="62"/>
-      <c r="R4" s="62"/>
-      <c r="S4" s="62"/>
-      <c r="T4" s="62"/>
-      <c r="U4" s="62"/>
-      <c r="V4" s="62"/>
-      <c r="W4" s="62"/>
-      <c r="X4" s="62"/>
-      <c r="Y4" s="62"/>
-      <c r="Z4" s="62"/>
-      <c r="AA4" s="62"/>
-      <c r="AB4" s="62"/>
-      <c r="AC4" s="62"/>
-      <c r="AD4" s="62"/>
-      <c r="AE4" s="62"/>
-      <c r="AF4" s="62"/>
-      <c r="AG4" s="62"/>
-      <c r="AH4" s="62"/>
-      <c r="AI4" s="62"/>
-      <c r="AJ4" s="62"/>
+      <c r="G4" s="62"/>
+      <c r="H4" s="63"/>
+      <c r="I4" s="64"/>
+      <c r="J4"/>
+      <c r="K4"/>
+      <c r="L4"/>
+      <c r="M4"/>
+      <c r="N4"/>
+      <c r="O4"/>
+      <c r="P4"/>
+      <c r="Q4"/>
+      <c r="R4"/>
+      <c r="S4"/>
+      <c r="T4"/>
+      <c r="U4"/>
+      <c r="V4"/>
+      <c r="W4"/>
+      <c r="X4"/>
+      <c r="Y4"/>
+      <c r="Z4"/>
+      <c r="AA4"/>
+      <c r="AB4"/>
+      <c r="AC4"/>
+      <c r="AD4"/>
+      <c r="AE4"/>
+      <c r="AF4"/>
+      <c r="AG4"/>
+      <c r="AH4"/>
+      <c r="AI4"/>
+      <c r="AJ4"/>
     </row>
     <row r="5" spans="1:36" s="4" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="27">
@@ -3473,45 +3521,45 @@
       <c r="C5" s="5">
         <v>1</v>
       </c>
-      <c r="D5" s="43" t="s">
+      <c r="D5" s="73" t="s">
+        <v>63</v>
+      </c>
+      <c r="E5" s="74"/>
+      <c r="F5" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="44"/>
-      <c r="F5" s="42" t="s">
-        <v>30</v>
-      </c>
-      <c r="G5" s="70" t="s">
-        <v>55</v>
-      </c>
-      <c r="H5" s="60"/>
-      <c r="I5" s="61"/>
-      <c r="J5" s="62"/>
-      <c r="K5" s="62"/>
-      <c r="L5" s="62"/>
-      <c r="M5" s="62"/>
-      <c r="N5" s="62"/>
-      <c r="O5" s="62"/>
-      <c r="P5" s="62"/>
-      <c r="Q5" s="62"/>
-      <c r="R5" s="62"/>
-      <c r="S5" s="62"/>
-      <c r="T5" s="62"/>
-      <c r="U5" s="62"/>
-      <c r="V5" s="62"/>
-      <c r="W5" s="62"/>
-      <c r="X5" s="62"/>
-      <c r="Y5" s="62"/>
-      <c r="Z5" s="62"/>
-      <c r="AA5" s="62"/>
-      <c r="AB5" s="62"/>
-      <c r="AC5" s="62"/>
-      <c r="AD5" s="62"/>
-      <c r="AE5" s="62"/>
-      <c r="AF5" s="62"/>
-      <c r="AG5" s="62"/>
-      <c r="AH5" s="62"/>
-      <c r="AI5" s="62"/>
-      <c r="AJ5" s="62"/>
+      <c r="G5" s="50" t="s">
+        <v>45</v>
+      </c>
+      <c r="H5" s="51"/>
+      <c r="I5" s="52"/>
+      <c r="J5"/>
+      <c r="K5"/>
+      <c r="L5"/>
+      <c r="M5"/>
+      <c r="N5"/>
+      <c r="O5"/>
+      <c r="P5"/>
+      <c r="Q5"/>
+      <c r="R5"/>
+      <c r="S5"/>
+      <c r="T5"/>
+      <c r="U5"/>
+      <c r="V5"/>
+      <c r="W5"/>
+      <c r="X5"/>
+      <c r="Y5"/>
+      <c r="Z5"/>
+      <c r="AA5"/>
+      <c r="AB5"/>
+      <c r="AC5"/>
+      <c r="AD5"/>
+      <c r="AE5"/>
+      <c r="AF5"/>
+      <c r="AG5"/>
+      <c r="AH5"/>
+      <c r="AI5"/>
+      <c r="AJ5"/>
     </row>
     <row r="6" spans="1:36" s="4" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5">
@@ -3523,45 +3571,45 @@
       <c r="C6" s="5">
         <v>2</v>
       </c>
-      <c r="D6" s="43" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" s="44"/>
-      <c r="F6" s="42" t="s">
-        <v>30</v>
-      </c>
-      <c r="G6" s="70" t="s">
-        <v>55</v>
-      </c>
-      <c r="H6" s="60"/>
-      <c r="I6" s="61"/>
-      <c r="J6" s="62"/>
-      <c r="K6" s="62"/>
-      <c r="L6" s="62"/>
-      <c r="M6" s="62"/>
-      <c r="N6" s="62"/>
-      <c r="O6" s="62"/>
-      <c r="P6" s="62"/>
-      <c r="Q6" s="62"/>
-      <c r="R6" s="62"/>
-      <c r="S6" s="62"/>
-      <c r="T6" s="62"/>
-      <c r="U6" s="62"/>
-      <c r="V6" s="62"/>
-      <c r="W6" s="62"/>
-      <c r="X6" s="62"/>
-      <c r="Y6" s="62"/>
-      <c r="Z6" s="62"/>
-      <c r="AA6" s="62"/>
-      <c r="AB6" s="62"/>
-      <c r="AC6" s="62"/>
-      <c r="AD6" s="62"/>
-      <c r="AE6" s="62"/>
-      <c r="AF6" s="62"/>
-      <c r="AG6" s="62"/>
-      <c r="AH6" s="62"/>
-      <c r="AI6" s="62"/>
-      <c r="AJ6" s="62"/>
+      <c r="D6" s="73" t="s">
+        <v>64</v>
+      </c>
+      <c r="E6" s="74"/>
+      <c r="F6" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="50" t="s">
+        <v>45</v>
+      </c>
+      <c r="H6" s="51"/>
+      <c r="I6" s="52"/>
+      <c r="J6"/>
+      <c r="K6"/>
+      <c r="L6"/>
+      <c r="M6"/>
+      <c r="N6"/>
+      <c r="O6"/>
+      <c r="P6"/>
+      <c r="Q6"/>
+      <c r="R6"/>
+      <c r="S6"/>
+      <c r="T6"/>
+      <c r="U6"/>
+      <c r="V6"/>
+      <c r="W6"/>
+      <c r="X6"/>
+      <c r="Y6"/>
+      <c r="Z6"/>
+      <c r="AA6"/>
+      <c r="AB6"/>
+      <c r="AC6"/>
+      <c r="AD6"/>
+      <c r="AE6"/>
+      <c r="AF6"/>
+      <c r="AG6"/>
+      <c r="AH6"/>
+      <c r="AI6"/>
+      <c r="AJ6"/>
     </row>
     <row r="7" spans="1:36" s="4" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5">
@@ -3573,45 +3621,45 @@
       <c r="C7" s="5">
         <v>3</v>
       </c>
-      <c r="D7" s="43" t="s">
-        <v>33</v>
-      </c>
-      <c r="E7" s="44"/>
-      <c r="F7" s="42" t="s">
-        <v>30</v>
-      </c>
-      <c r="G7" s="70" t="s">
-        <v>56</v>
-      </c>
-      <c r="H7" s="60"/>
-      <c r="I7" s="61"/>
-      <c r="J7" s="62"/>
-      <c r="K7" s="62"/>
-      <c r="L7" s="62"/>
-      <c r="M7" s="62"/>
-      <c r="N7" s="62"/>
-      <c r="O7" s="62"/>
-      <c r="P7" s="62"/>
-      <c r="Q7" s="62"/>
-      <c r="R7" s="62"/>
-      <c r="S7" s="62"/>
-      <c r="T7" s="62"/>
-      <c r="U7" s="62"/>
-      <c r="V7" s="62"/>
-      <c r="W7" s="62"/>
-      <c r="X7" s="62"/>
-      <c r="Y7" s="62"/>
-      <c r="Z7" s="62"/>
-      <c r="AA7" s="62"/>
-      <c r="AB7" s="62"/>
-      <c r="AC7" s="62"/>
-      <c r="AD7" s="62"/>
-      <c r="AE7" s="62"/>
-      <c r="AF7" s="62"/>
-      <c r="AG7" s="62"/>
-      <c r="AH7" s="62"/>
-      <c r="AI7" s="62"/>
-      <c r="AJ7" s="62"/>
+      <c r="D7" s="73" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="74"/>
+      <c r="F7" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" s="50" t="s">
+        <v>46</v>
+      </c>
+      <c r="H7" s="51"/>
+      <c r="I7" s="52"/>
+      <c r="J7"/>
+      <c r="K7"/>
+      <c r="L7"/>
+      <c r="M7"/>
+      <c r="N7"/>
+      <c r="O7"/>
+      <c r="P7"/>
+      <c r="Q7"/>
+      <c r="R7"/>
+      <c r="S7"/>
+      <c r="T7"/>
+      <c r="U7"/>
+      <c r="V7"/>
+      <c r="W7"/>
+      <c r="X7"/>
+      <c r="Y7"/>
+      <c r="Z7"/>
+      <c r="AA7"/>
+      <c r="AB7"/>
+      <c r="AC7"/>
+      <c r="AD7"/>
+      <c r="AE7"/>
+      <c r="AF7"/>
+      <c r="AG7"/>
+      <c r="AH7"/>
+      <c r="AI7"/>
+      <c r="AJ7"/>
     </row>
     <row r="8" spans="1:36" s="4" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5">
@@ -3623,45 +3671,45 @@
       <c r="C8" s="5">
         <v>4</v>
       </c>
-      <c r="D8" s="43" t="s">
-        <v>34</v>
-      </c>
-      <c r="E8" s="44"/>
-      <c r="F8" s="42" t="s">
-        <v>30</v>
-      </c>
-      <c r="G8" s="70" t="s">
-        <v>55</v>
-      </c>
-      <c r="H8" s="60"/>
-      <c r="I8" s="61"/>
-      <c r="J8" s="62"/>
-      <c r="K8" s="62"/>
-      <c r="L8" s="62"/>
-      <c r="M8" s="62"/>
-      <c r="N8" s="62"/>
-      <c r="O8" s="62"/>
-      <c r="P8" s="62"/>
-      <c r="Q8" s="62"/>
-      <c r="R8" s="62"/>
-      <c r="S8" s="62"/>
-      <c r="T8" s="62"/>
-      <c r="U8" s="62"/>
-      <c r="V8" s="62"/>
-      <c r="W8" s="62"/>
-      <c r="X8" s="62"/>
-      <c r="Y8" s="62"/>
-      <c r="Z8" s="62"/>
-      <c r="AA8" s="62"/>
-      <c r="AB8" s="62"/>
-      <c r="AC8" s="62"/>
-      <c r="AD8" s="62"/>
-      <c r="AE8" s="62"/>
-      <c r="AF8" s="62"/>
-      <c r="AG8" s="62"/>
-      <c r="AH8" s="62"/>
-      <c r="AI8" s="62"/>
-      <c r="AJ8" s="62"/>
+      <c r="D8" s="73" t="s">
+        <v>65</v>
+      </c>
+      <c r="E8" s="74"/>
+      <c r="F8" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" s="50" t="s">
+        <v>45</v>
+      </c>
+      <c r="H8" s="51"/>
+      <c r="I8" s="52"/>
+      <c r="J8"/>
+      <c r="K8"/>
+      <c r="L8"/>
+      <c r="M8"/>
+      <c r="N8"/>
+      <c r="O8"/>
+      <c r="P8"/>
+      <c r="Q8"/>
+      <c r="R8"/>
+      <c r="S8"/>
+      <c r="T8"/>
+      <c r="U8"/>
+      <c r="V8"/>
+      <c r="W8"/>
+      <c r="X8"/>
+      <c r="Y8"/>
+      <c r="Z8"/>
+      <c r="AA8"/>
+      <c r="AB8"/>
+      <c r="AC8"/>
+      <c r="AD8"/>
+      <c r="AE8"/>
+      <c r="AF8"/>
+      <c r="AG8"/>
+      <c r="AH8"/>
+      <c r="AI8"/>
+      <c r="AJ8"/>
     </row>
     <row r="9" spans="1:36" s="4" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5">
@@ -3673,45 +3721,45 @@
       <c r="C9" s="5">
         <v>5</v>
       </c>
-      <c r="D9" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="E9" s="44"/>
-      <c r="F9" s="42" t="s">
+      <c r="D9" s="73" t="s">
         <v>30</v>
       </c>
-      <c r="G9" s="70" t="s">
-        <v>55</v>
-      </c>
-      <c r="H9" s="60"/>
-      <c r="I9" s="61"/>
-      <c r="J9" s="62"/>
-      <c r="K9" s="62"/>
-      <c r="L9" s="62"/>
-      <c r="M9" s="62"/>
-      <c r="N9" s="62"/>
-      <c r="O9" s="62"/>
-      <c r="P9" s="62"/>
-      <c r="Q9" s="62"/>
-      <c r="R9" s="62"/>
-      <c r="S9" s="62"/>
-      <c r="T9" s="62"/>
-      <c r="U9" s="62"/>
-      <c r="V9" s="62"/>
-      <c r="W9" s="62"/>
-      <c r="X9" s="62"/>
-      <c r="Y9" s="62"/>
-      <c r="Z9" s="62"/>
-      <c r="AA9" s="62"/>
-      <c r="AB9" s="62"/>
-      <c r="AC9" s="62"/>
-      <c r="AD9" s="62"/>
-      <c r="AE9" s="62"/>
-      <c r="AF9" s="62"/>
-      <c r="AG9" s="62"/>
-      <c r="AH9" s="62"/>
-      <c r="AI9" s="62"/>
-      <c r="AJ9" s="62"/>
+      <c r="E9" s="74"/>
+      <c r="F9" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" s="50" t="s">
+        <v>45</v>
+      </c>
+      <c r="H9" s="51"/>
+      <c r="I9" s="52"/>
+      <c r="J9"/>
+      <c r="K9"/>
+      <c r="L9"/>
+      <c r="M9"/>
+      <c r="N9"/>
+      <c r="O9"/>
+      <c r="P9"/>
+      <c r="Q9"/>
+      <c r="R9"/>
+      <c r="S9"/>
+      <c r="T9"/>
+      <c r="U9"/>
+      <c r="V9"/>
+      <c r="W9"/>
+      <c r="X9"/>
+      <c r="Y9"/>
+      <c r="Z9"/>
+      <c r="AA9"/>
+      <c r="AB9"/>
+      <c r="AC9"/>
+      <c r="AD9"/>
+      <c r="AE9"/>
+      <c r="AF9"/>
+      <c r="AG9"/>
+      <c r="AH9"/>
+      <c r="AI9"/>
+      <c r="AJ9"/>
     </row>
     <row r="10" spans="1:36" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A10" s="16"/>
@@ -3725,7 +3773,7 @@
         <v>5</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F10" s="19" t="s">
         <v>2</v>
@@ -3735,77 +3783,77 @@
       </c>
       <c r="H10" s="54"/>
       <c r="I10" s="55"/>
-      <c r="J10" s="62"/>
-      <c r="K10" s="62"/>
-      <c r="L10" s="62"/>
-      <c r="M10" s="62"/>
-      <c r="N10" s="62"/>
-      <c r="O10" s="62"/>
-      <c r="P10" s="62"/>
-      <c r="Q10" s="62"/>
-      <c r="R10" s="62"/>
-      <c r="S10" s="62"/>
-      <c r="T10" s="62"/>
-      <c r="U10" s="62"/>
-      <c r="V10" s="62"/>
-      <c r="W10" s="62"/>
-      <c r="X10" s="62"/>
-      <c r="Y10" s="62"/>
-      <c r="Z10" s="62"/>
-      <c r="AA10" s="62"/>
-      <c r="AB10" s="62"/>
-      <c r="AC10" s="62"/>
-      <c r="AD10" s="62"/>
-      <c r="AE10" s="62"/>
-      <c r="AF10" s="62"/>
-      <c r="AG10" s="62"/>
-      <c r="AH10" s="62"/>
-      <c r="AI10" s="62"/>
-      <c r="AJ10" s="62"/>
+      <c r="J10"/>
+      <c r="K10"/>
+      <c r="L10"/>
+      <c r="M10"/>
+      <c r="N10"/>
+      <c r="O10"/>
+      <c r="P10"/>
+      <c r="Q10"/>
+      <c r="R10"/>
+      <c r="S10"/>
+      <c r="T10"/>
+      <c r="U10"/>
+      <c r="V10"/>
+      <c r="W10"/>
+      <c r="X10"/>
+      <c r="Y10"/>
+      <c r="Z10"/>
+      <c r="AA10"/>
+      <c r="AB10"/>
+      <c r="AC10"/>
+      <c r="AD10"/>
+      <c r="AE10"/>
+      <c r="AF10"/>
+      <c r="AG10"/>
+      <c r="AH10"/>
+      <c r="AI10"/>
+      <c r="AJ10"/>
     </row>
     <row r="11" spans="1:36" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="49" t="s">
+      <c r="B11" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="50"/>
-      <c r="D11" s="45" t="s">
+      <c r="C11" s="59"/>
+      <c r="D11" s="60" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="46"/>
+      <c r="E11" s="61"/>
       <c r="F11" s="21"/>
-      <c r="G11" s="56"/>
-      <c r="H11" s="57"/>
-      <c r="I11" s="58"/>
-      <c r="J11" s="62"/>
-      <c r="K11" s="62"/>
-      <c r="L11" s="62"/>
-      <c r="M11" s="62"/>
-      <c r="N11" s="62"/>
-      <c r="O11" s="62"/>
-      <c r="P11" s="62"/>
-      <c r="Q11" s="62"/>
-      <c r="R11" s="62"/>
-      <c r="S11" s="62"/>
-      <c r="T11" s="62"/>
-      <c r="U11" s="62"/>
-      <c r="V11" s="62"/>
-      <c r="W11" s="62"/>
-      <c r="X11" s="62"/>
-      <c r="Y11" s="62"/>
-      <c r="Z11" s="62"/>
-      <c r="AA11" s="62"/>
-      <c r="AB11" s="62"/>
-      <c r="AC11" s="62"/>
-      <c r="AD11" s="62"/>
-      <c r="AE11" s="62"/>
-      <c r="AF11" s="62"/>
-      <c r="AG11" s="62"/>
-      <c r="AH11" s="62"/>
-      <c r="AI11" s="62"/>
-      <c r="AJ11" s="62"/>
+      <c r="G11" s="62"/>
+      <c r="H11" s="63"/>
+      <c r="I11" s="64"/>
+      <c r="J11"/>
+      <c r="K11"/>
+      <c r="L11"/>
+      <c r="M11"/>
+      <c r="N11"/>
+      <c r="O11"/>
+      <c r="P11"/>
+      <c r="Q11"/>
+      <c r="R11"/>
+      <c r="S11"/>
+      <c r="T11"/>
+      <c r="U11"/>
+      <c r="V11"/>
+      <c r="W11"/>
+      <c r="X11"/>
+      <c r="Y11"/>
+      <c r="Z11"/>
+      <c r="AA11"/>
+      <c r="AB11"/>
+      <c r="AC11"/>
+      <c r="AD11"/>
+      <c r="AE11"/>
+      <c r="AF11"/>
+      <c r="AG11"/>
+      <c r="AH11"/>
+      <c r="AI11"/>
+      <c r="AJ11"/>
     </row>
     <row r="12" spans="1:36" s="4" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5">
@@ -3817,45 +3865,45 @@
       <c r="C12" s="5">
         <v>1</v>
       </c>
-      <c r="D12" s="51" t="s">
-        <v>39</v>
-      </c>
-      <c r="E12" s="52"/>
-      <c r="F12" s="42" t="s">
-        <v>30</v>
-      </c>
-      <c r="G12" s="70" t="s">
-        <v>55</v>
-      </c>
-      <c r="H12" s="60"/>
-      <c r="I12" s="61"/>
-      <c r="J12" s="62"/>
-      <c r="K12" s="62"/>
-      <c r="L12" s="62"/>
-      <c r="M12" s="62"/>
-      <c r="N12" s="62"/>
-      <c r="O12" s="62"/>
-      <c r="P12" s="62"/>
-      <c r="Q12" s="62"/>
-      <c r="R12" s="62"/>
-      <c r="S12" s="62"/>
-      <c r="T12" s="62"/>
-      <c r="U12" s="62"/>
-      <c r="V12" s="62"/>
-      <c r="W12" s="62"/>
-      <c r="X12" s="62"/>
-      <c r="Y12" s="62"/>
-      <c r="Z12" s="62"/>
-      <c r="AA12" s="62"/>
-      <c r="AB12" s="62"/>
-      <c r="AC12" s="62"/>
-      <c r="AD12" s="62"/>
-      <c r="AE12" s="62"/>
-      <c r="AF12" s="62"/>
-      <c r="AG12" s="62"/>
-      <c r="AH12" s="62"/>
-      <c r="AI12" s="62"/>
-      <c r="AJ12" s="62"/>
+      <c r="D12" s="56" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" s="57"/>
+      <c r="F12" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="G12" s="50" t="s">
+        <v>45</v>
+      </c>
+      <c r="H12" s="51"/>
+      <c r="I12" s="52"/>
+      <c r="J12"/>
+      <c r="K12"/>
+      <c r="L12"/>
+      <c r="M12"/>
+      <c r="N12"/>
+      <c r="O12"/>
+      <c r="P12"/>
+      <c r="Q12"/>
+      <c r="R12"/>
+      <c r="S12"/>
+      <c r="T12"/>
+      <c r="U12"/>
+      <c r="V12"/>
+      <c r="W12"/>
+      <c r="X12"/>
+      <c r="Y12"/>
+      <c r="Z12"/>
+      <c r="AA12"/>
+      <c r="AB12"/>
+      <c r="AC12"/>
+      <c r="AD12"/>
+      <c r="AE12"/>
+      <c r="AF12"/>
+      <c r="AG12"/>
+      <c r="AH12"/>
+      <c r="AI12"/>
+      <c r="AJ12"/>
     </row>
     <row r="13" spans="1:36" s="4" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5">
@@ -3867,45 +3915,45 @@
       <c r="C13" s="5">
         <v>2</v>
       </c>
-      <c r="D13" s="51" t="s">
-        <v>40</v>
-      </c>
-      <c r="E13" s="52"/>
-      <c r="F13" s="42" t="s">
-        <v>30</v>
-      </c>
-      <c r="G13" s="70" t="s">
-        <v>55</v>
-      </c>
-      <c r="H13" s="60"/>
-      <c r="I13" s="61"/>
-      <c r="J13" s="62"/>
-      <c r="K13" s="62"/>
-      <c r="L13" s="62"/>
-      <c r="M13" s="62"/>
-      <c r="N13" s="62"/>
-      <c r="O13" s="62"/>
-      <c r="P13" s="62"/>
-      <c r="Q13" s="62"/>
-      <c r="R13" s="62"/>
-      <c r="S13" s="62"/>
-      <c r="T13" s="62"/>
-      <c r="U13" s="62"/>
-      <c r="V13" s="62"/>
-      <c r="W13" s="62"/>
-      <c r="X13" s="62"/>
-      <c r="Y13" s="62"/>
-      <c r="Z13" s="62"/>
-      <c r="AA13" s="62"/>
-      <c r="AB13" s="62"/>
-      <c r="AC13" s="62"/>
-      <c r="AD13" s="62"/>
-      <c r="AE13" s="62"/>
-      <c r="AF13" s="62"/>
-      <c r="AG13" s="62"/>
-      <c r="AH13" s="62"/>
-      <c r="AI13" s="62"/>
-      <c r="AJ13" s="62"/>
+      <c r="D13" s="56" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" s="57"/>
+      <c r="F13" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="G13" s="50" t="s">
+        <v>45</v>
+      </c>
+      <c r="H13" s="51"/>
+      <c r="I13" s="52"/>
+      <c r="J13"/>
+      <c r="K13"/>
+      <c r="L13"/>
+      <c r="M13"/>
+      <c r="N13"/>
+      <c r="O13"/>
+      <c r="P13"/>
+      <c r="Q13"/>
+      <c r="R13"/>
+      <c r="S13"/>
+      <c r="T13"/>
+      <c r="U13"/>
+      <c r="V13"/>
+      <c r="W13"/>
+      <c r="X13"/>
+      <c r="Y13"/>
+      <c r="Z13"/>
+      <c r="AA13"/>
+      <c r="AB13"/>
+      <c r="AC13"/>
+      <c r="AD13"/>
+      <c r="AE13"/>
+      <c r="AF13"/>
+      <c r="AG13"/>
+      <c r="AH13"/>
+      <c r="AI13"/>
+      <c r="AJ13"/>
     </row>
     <row r="14" spans="1:36" s="4" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5">
@@ -3917,45 +3965,45 @@
       <c r="C14" s="5">
         <v>3</v>
       </c>
-      <c r="D14" s="59" t="s">
-        <v>41</v>
-      </c>
-      <c r="E14" s="61"/>
-      <c r="F14" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="G14" s="70" t="s">
-        <v>55</v>
-      </c>
-      <c r="H14" s="60"/>
-      <c r="I14" s="61"/>
-      <c r="J14" s="62"/>
-      <c r="K14" s="62"/>
-      <c r="L14" s="62"/>
-      <c r="M14" s="62"/>
-      <c r="N14" s="62"/>
-      <c r="O14" s="62"/>
-      <c r="P14" s="62"/>
-      <c r="Q14" s="62"/>
-      <c r="R14" s="62"/>
-      <c r="S14" s="62"/>
-      <c r="T14" s="62"/>
-      <c r="U14" s="62"/>
-      <c r="V14" s="62"/>
-      <c r="W14" s="62"/>
-      <c r="X14" s="62"/>
-      <c r="Y14" s="62"/>
-      <c r="Z14" s="62"/>
-      <c r="AA14" s="62"/>
-      <c r="AB14" s="62"/>
-      <c r="AC14" s="62"/>
-      <c r="AD14" s="62"/>
-      <c r="AE14" s="62"/>
-      <c r="AF14" s="62"/>
-      <c r="AG14" s="62"/>
-      <c r="AH14" s="62"/>
-      <c r="AI14" s="62"/>
-      <c r="AJ14" s="62"/>
+      <c r="D14" s="67" t="s">
+        <v>62</v>
+      </c>
+      <c r="E14" s="52"/>
+      <c r="F14" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="G14" s="50" t="s">
+        <v>45</v>
+      </c>
+      <c r="H14" s="51"/>
+      <c r="I14" s="52"/>
+      <c r="J14"/>
+      <c r="K14"/>
+      <c r="L14"/>
+      <c r="M14"/>
+      <c r="N14"/>
+      <c r="O14"/>
+      <c r="P14"/>
+      <c r="Q14"/>
+      <c r="R14"/>
+      <c r="S14"/>
+      <c r="T14"/>
+      <c r="U14"/>
+      <c r="V14"/>
+      <c r="W14"/>
+      <c r="X14"/>
+      <c r="Y14"/>
+      <c r="Z14"/>
+      <c r="AA14"/>
+      <c r="AB14"/>
+      <c r="AC14"/>
+      <c r="AD14"/>
+      <c r="AE14"/>
+      <c r="AF14"/>
+      <c r="AG14"/>
+      <c r="AH14"/>
+      <c r="AI14"/>
+      <c r="AJ14"/>
     </row>
     <row r="15" spans="1:36" s="4" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5">
@@ -3967,45 +4015,45 @@
       <c r="C15" s="5">
         <v>4</v>
       </c>
-      <c r="D15" s="67" t="s">
-        <v>43</v>
-      </c>
-      <c r="E15" s="68"/>
-      <c r="F15" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="G15" s="70" t="s">
-        <v>55</v>
-      </c>
-      <c r="H15" s="60"/>
-      <c r="I15" s="61"/>
-      <c r="J15" s="62"/>
-      <c r="K15" s="62"/>
-      <c r="L15" s="62"/>
-      <c r="M15" s="62"/>
-      <c r="N15" s="62"/>
-      <c r="O15" s="62"/>
-      <c r="P15" s="62"/>
-      <c r="Q15" s="62"/>
-      <c r="R15" s="62"/>
-      <c r="S15" s="62"/>
-      <c r="T15" s="62"/>
-      <c r="U15" s="62"/>
-      <c r="V15" s="62"/>
-      <c r="W15" s="62"/>
-      <c r="X15" s="62"/>
-      <c r="Y15" s="62"/>
-      <c r="Z15" s="62"/>
-      <c r="AA15" s="62"/>
-      <c r="AB15" s="62"/>
-      <c r="AC15" s="62"/>
-      <c r="AD15" s="62"/>
-      <c r="AE15" s="62"/>
-      <c r="AF15" s="62"/>
-      <c r="AG15" s="62"/>
-      <c r="AH15" s="62"/>
-      <c r="AI15" s="62"/>
-      <c r="AJ15" s="62"/>
+      <c r="D15" s="65" t="s">
+        <v>71</v>
+      </c>
+      <c r="E15" s="66"/>
+      <c r="F15" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="G15" s="50" t="s">
+        <v>45</v>
+      </c>
+      <c r="H15" s="51"/>
+      <c r="I15" s="52"/>
+      <c r="J15"/>
+      <c r="K15"/>
+      <c r="L15"/>
+      <c r="M15"/>
+      <c r="N15"/>
+      <c r="O15"/>
+      <c r="P15"/>
+      <c r="Q15"/>
+      <c r="R15"/>
+      <c r="S15"/>
+      <c r="T15"/>
+      <c r="U15"/>
+      <c r="V15"/>
+      <c r="W15"/>
+      <c r="X15"/>
+      <c r="Y15"/>
+      <c r="Z15"/>
+      <c r="AA15"/>
+      <c r="AB15"/>
+      <c r="AC15"/>
+      <c r="AD15"/>
+      <c r="AE15"/>
+      <c r="AF15"/>
+      <c r="AG15"/>
+      <c r="AH15"/>
+      <c r="AI15"/>
+      <c r="AJ15"/>
     </row>
     <row r="16" spans="1:36" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A16" s="16"/>
@@ -4019,7 +4067,7 @@
         <v>5</v>
       </c>
       <c r="E16" s="22" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="F16" s="19" t="s">
         <v>2</v>
@@ -4029,77 +4077,77 @@
       </c>
       <c r="H16" s="54"/>
       <c r="I16" s="55"/>
-      <c r="J16" s="62"/>
-      <c r="K16" s="62"/>
-      <c r="L16" s="62"/>
-      <c r="M16" s="62"/>
-      <c r="N16" s="62"/>
-      <c r="O16" s="62"/>
-      <c r="P16" s="62"/>
-      <c r="Q16" s="62"/>
-      <c r="R16" s="62"/>
-      <c r="S16" s="62"/>
-      <c r="T16" s="62"/>
-      <c r="U16" s="62"/>
-      <c r="V16" s="62"/>
-      <c r="W16" s="62"/>
-      <c r="X16" s="62"/>
-      <c r="Y16" s="62"/>
-      <c r="Z16" s="62"/>
-      <c r="AA16" s="62"/>
-      <c r="AB16" s="62"/>
-      <c r="AC16" s="62"/>
-      <c r="AD16" s="62"/>
-      <c r="AE16" s="62"/>
-      <c r="AF16" s="62"/>
-      <c r="AG16" s="62"/>
-      <c r="AH16" s="62"/>
-      <c r="AI16" s="62"/>
-      <c r="AJ16" s="62"/>
+      <c r="J16"/>
+      <c r="K16"/>
+      <c r="L16"/>
+      <c r="M16"/>
+      <c r="N16"/>
+      <c r="O16"/>
+      <c r="P16"/>
+      <c r="Q16"/>
+      <c r="R16"/>
+      <c r="S16"/>
+      <c r="T16"/>
+      <c r="U16"/>
+      <c r="V16"/>
+      <c r="W16"/>
+      <c r="X16"/>
+      <c r="Y16"/>
+      <c r="Z16"/>
+      <c r="AA16"/>
+      <c r="AB16"/>
+      <c r="AC16"/>
+      <c r="AD16"/>
+      <c r="AE16"/>
+      <c r="AF16"/>
+      <c r="AG16"/>
+      <c r="AH16"/>
+      <c r="AI16"/>
+      <c r="AJ16"/>
     </row>
     <row r="17" spans="1:36" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="49" t="s">
+      <c r="B17" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="50"/>
-      <c r="D17" s="45" t="s">
+      <c r="C17" s="59"/>
+      <c r="D17" s="60" t="s">
         <v>17</v>
       </c>
-      <c r="E17" s="46"/>
+      <c r="E17" s="61"/>
       <c r="F17" s="21"/>
-      <c r="G17" s="56"/>
-      <c r="H17" s="57"/>
-      <c r="I17" s="58"/>
-      <c r="J17" s="62"/>
-      <c r="K17" s="62"/>
-      <c r="L17" s="62"/>
-      <c r="M17" s="62"/>
-      <c r="N17" s="62"/>
-      <c r="O17" s="62"/>
-      <c r="P17" s="62"/>
-      <c r="Q17" s="62"/>
-      <c r="R17" s="62"/>
-      <c r="S17" s="62"/>
-      <c r="T17" s="62"/>
-      <c r="U17" s="62"/>
-      <c r="V17" s="62"/>
-      <c r="W17" s="62"/>
-      <c r="X17" s="62"/>
-      <c r="Y17" s="62"/>
-      <c r="Z17" s="62"/>
-      <c r="AA17" s="62"/>
-      <c r="AB17" s="62"/>
-      <c r="AC17" s="62"/>
-      <c r="AD17" s="62"/>
-      <c r="AE17" s="62"/>
-      <c r="AF17" s="62"/>
-      <c r="AG17" s="62"/>
-      <c r="AH17" s="62"/>
-      <c r="AI17" s="62"/>
-      <c r="AJ17" s="62"/>
+      <c r="G17" s="62"/>
+      <c r="H17" s="63"/>
+      <c r="I17" s="64"/>
+      <c r="J17"/>
+      <c r="K17"/>
+      <c r="L17"/>
+      <c r="M17"/>
+      <c r="N17"/>
+      <c r="O17"/>
+      <c r="P17"/>
+      <c r="Q17"/>
+      <c r="R17"/>
+      <c r="S17"/>
+      <c r="T17"/>
+      <c r="U17"/>
+      <c r="V17"/>
+      <c r="W17"/>
+      <c r="X17"/>
+      <c r="Y17"/>
+      <c r="Z17"/>
+      <c r="AA17"/>
+      <c r="AB17"/>
+      <c r="AC17"/>
+      <c r="AD17"/>
+      <c r="AE17"/>
+      <c r="AF17"/>
+      <c r="AG17"/>
+      <c r="AH17"/>
+      <c r="AI17"/>
+      <c r="AJ17"/>
     </row>
     <row r="18" spans="1:36" s="4" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="5">
@@ -4111,45 +4159,45 @@
       <c r="C18" s="5">
         <v>1</v>
       </c>
-      <c r="D18" s="51" t="s">
-        <v>47</v>
-      </c>
-      <c r="E18" s="52"/>
-      <c r="F18" s="42" t="s">
-        <v>30</v>
-      </c>
-      <c r="G18" s="70" t="s">
-        <v>55</v>
-      </c>
-      <c r="H18" s="60"/>
-      <c r="I18" s="61"/>
-      <c r="J18" s="62"/>
-      <c r="K18" s="62"/>
-      <c r="L18" s="62"/>
-      <c r="M18" s="62"/>
-      <c r="N18" s="62"/>
-      <c r="O18" s="62"/>
-      <c r="P18" s="62"/>
-      <c r="Q18" s="62"/>
-      <c r="R18" s="62"/>
-      <c r="S18" s="62"/>
-      <c r="T18" s="62"/>
-      <c r="U18" s="62"/>
-      <c r="V18" s="62"/>
-      <c r="W18" s="62"/>
-      <c r="X18" s="62"/>
-      <c r="Y18" s="62"/>
-      <c r="Z18" s="62"/>
-      <c r="AA18" s="62"/>
-      <c r="AB18" s="62"/>
-      <c r="AC18" s="62"/>
-      <c r="AD18" s="62"/>
-      <c r="AE18" s="62"/>
-      <c r="AF18" s="62"/>
-      <c r="AG18" s="62"/>
-      <c r="AH18" s="62"/>
-      <c r="AI18" s="62"/>
-      <c r="AJ18" s="62"/>
+      <c r="D18" s="56" t="s">
+        <v>40</v>
+      </c>
+      <c r="E18" s="57"/>
+      <c r="F18" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="G18" s="50" t="s">
+        <v>45</v>
+      </c>
+      <c r="H18" s="51"/>
+      <c r="I18" s="52"/>
+      <c r="J18"/>
+      <c r="K18"/>
+      <c r="L18"/>
+      <c r="M18"/>
+      <c r="N18"/>
+      <c r="O18"/>
+      <c r="P18"/>
+      <c r="Q18"/>
+      <c r="R18"/>
+      <c r="S18"/>
+      <c r="T18"/>
+      <c r="U18"/>
+      <c r="V18"/>
+      <c r="W18"/>
+      <c r="X18"/>
+      <c r="Y18"/>
+      <c r="Z18"/>
+      <c r="AA18"/>
+      <c r="AB18"/>
+      <c r="AC18"/>
+      <c r="AD18"/>
+      <c r="AE18"/>
+      <c r="AF18"/>
+      <c r="AG18"/>
+      <c r="AH18"/>
+      <c r="AI18"/>
+      <c r="AJ18"/>
     </row>
     <row r="19" spans="1:36" s="4" customFormat="1" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="5">
@@ -4161,45 +4209,45 @@
       <c r="C19" s="5">
         <v>2</v>
       </c>
-      <c r="D19" s="51" t="s">
-        <v>49</v>
-      </c>
-      <c r="E19" s="52"/>
-      <c r="F19" s="42" t="s">
-        <v>30</v>
-      </c>
-      <c r="G19" s="70" t="s">
-        <v>55</v>
-      </c>
-      <c r="H19" s="60"/>
-      <c r="I19" s="61"/>
-      <c r="J19" s="62"/>
-      <c r="K19" s="62"/>
-      <c r="L19" s="62"/>
-      <c r="M19" s="62"/>
-      <c r="N19" s="62"/>
-      <c r="O19" s="62"/>
-      <c r="P19" s="62"/>
-      <c r="Q19" s="62"/>
-      <c r="R19" s="62"/>
-      <c r="S19" s="62"/>
-      <c r="T19" s="62"/>
-      <c r="U19" s="62"/>
-      <c r="V19" s="62"/>
-      <c r="W19" s="62"/>
-      <c r="X19" s="62"/>
-      <c r="Y19" s="62"/>
-      <c r="Z19" s="62"/>
-      <c r="AA19" s="62"/>
-      <c r="AB19" s="62"/>
-      <c r="AC19" s="62"/>
-      <c r="AD19" s="62"/>
-      <c r="AE19" s="62"/>
-      <c r="AF19" s="62"/>
-      <c r="AG19" s="62"/>
-      <c r="AH19" s="62"/>
-      <c r="AI19" s="62"/>
-      <c r="AJ19" s="62"/>
+      <c r="D19" s="56" t="s">
+        <v>42</v>
+      </c>
+      <c r="E19" s="57"/>
+      <c r="F19" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="G19" s="50" t="s">
+        <v>45</v>
+      </c>
+      <c r="H19" s="51"/>
+      <c r="I19" s="52"/>
+      <c r="J19"/>
+      <c r="K19"/>
+      <c r="L19"/>
+      <c r="M19"/>
+      <c r="N19"/>
+      <c r="O19"/>
+      <c r="P19"/>
+      <c r="Q19"/>
+      <c r="R19"/>
+      <c r="S19"/>
+      <c r="T19"/>
+      <c r="U19"/>
+      <c r="V19"/>
+      <c r="W19"/>
+      <c r="X19"/>
+      <c r="Y19"/>
+      <c r="Z19"/>
+      <c r="AA19"/>
+      <c r="AB19"/>
+      <c r="AC19"/>
+      <c r="AD19"/>
+      <c r="AE19"/>
+      <c r="AF19"/>
+      <c r="AG19"/>
+      <c r="AH19"/>
+      <c r="AI19"/>
+      <c r="AJ19"/>
     </row>
     <row r="20" spans="1:36" s="4" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="5">
@@ -4211,45 +4259,45 @@
       <c r="C20" s="5">
         <v>3</v>
       </c>
-      <c r="D20" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="E20" s="52"/>
-      <c r="F20" s="42" t="s">
-        <v>30</v>
-      </c>
-      <c r="G20" s="70" t="s">
-        <v>55</v>
-      </c>
-      <c r="H20" s="60"/>
-      <c r="I20" s="61"/>
-      <c r="J20" s="62"/>
-      <c r="K20" s="62"/>
-      <c r="L20" s="62"/>
-      <c r="M20" s="62"/>
-      <c r="N20" s="62"/>
-      <c r="O20" s="62"/>
-      <c r="P20" s="62"/>
-      <c r="Q20" s="62"/>
-      <c r="R20" s="62"/>
-      <c r="S20" s="62"/>
-      <c r="T20" s="62"/>
-      <c r="U20" s="62"/>
-      <c r="V20" s="62"/>
-      <c r="W20" s="62"/>
-      <c r="X20" s="62"/>
-      <c r="Y20" s="62"/>
-      <c r="Z20" s="62"/>
-      <c r="AA20" s="62"/>
-      <c r="AB20" s="62"/>
-      <c r="AC20" s="62"/>
-      <c r="AD20" s="62"/>
-      <c r="AE20" s="62"/>
-      <c r="AF20" s="62"/>
-      <c r="AG20" s="62"/>
-      <c r="AH20" s="62"/>
-      <c r="AI20" s="62"/>
-      <c r="AJ20" s="62"/>
+      <c r="D20" s="56" t="s">
+        <v>66</v>
+      </c>
+      <c r="E20" s="57"/>
+      <c r="F20" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="G20" s="50" t="s">
+        <v>45</v>
+      </c>
+      <c r="H20" s="51"/>
+      <c r="I20" s="52"/>
+      <c r="J20"/>
+      <c r="K20"/>
+      <c r="L20"/>
+      <c r="M20"/>
+      <c r="N20"/>
+      <c r="O20"/>
+      <c r="P20"/>
+      <c r="Q20"/>
+      <c r="R20"/>
+      <c r="S20"/>
+      <c r="T20"/>
+      <c r="U20"/>
+      <c r="V20"/>
+      <c r="W20"/>
+      <c r="X20"/>
+      <c r="Y20"/>
+      <c r="Z20"/>
+      <c r="AA20"/>
+      <c r="AB20"/>
+      <c r="AC20"/>
+      <c r="AD20"/>
+      <c r="AE20"/>
+      <c r="AF20"/>
+      <c r="AG20"/>
+      <c r="AH20"/>
+      <c r="AI20"/>
+      <c r="AJ20"/>
     </row>
     <row r="21" spans="1:36" s="4" customFormat="1" ht="71.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="5">
@@ -4261,88 +4309,88 @@
       <c r="C21" s="5">
         <v>4</v>
       </c>
-      <c r="D21" s="51" t="s">
-        <v>51</v>
-      </c>
-      <c r="E21" s="52"/>
-      <c r="F21" s="42" t="s">
-        <v>52</v>
-      </c>
-      <c r="G21" s="70" t="s">
-        <v>55</v>
-      </c>
-      <c r="H21" s="60"/>
-      <c r="I21" s="61"/>
-      <c r="J21" s="62"/>
-      <c r="K21" s="62"/>
-      <c r="L21" s="62"/>
-      <c r="M21" s="62"/>
-      <c r="N21" s="62"/>
-      <c r="O21" s="62"/>
-      <c r="P21" s="62"/>
-      <c r="Q21" s="62"/>
-      <c r="R21" s="62"/>
-      <c r="S21" s="62"/>
-      <c r="T21" s="62"/>
-      <c r="U21" s="62"/>
-      <c r="V21" s="62"/>
-      <c r="W21" s="62"/>
-      <c r="X21" s="62"/>
-      <c r="Y21" s="62"/>
-      <c r="Z21" s="62"/>
-      <c r="AA21" s="62"/>
-      <c r="AB21" s="62"/>
-      <c r="AC21" s="62"/>
-      <c r="AD21" s="62"/>
-      <c r="AE21" s="62"/>
-      <c r="AF21" s="62"/>
-      <c r="AG21" s="62"/>
-      <c r="AH21" s="62"/>
-      <c r="AI21" s="62"/>
-      <c r="AJ21" s="62"/>
+      <c r="D21" s="56" t="s">
+        <v>70</v>
+      </c>
+      <c r="E21" s="57"/>
+      <c r="F21" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="G21" s="50" t="s">
+        <v>45</v>
+      </c>
+      <c r="H21" s="51"/>
+      <c r="I21" s="52"/>
+      <c r="J21"/>
+      <c r="K21"/>
+      <c r="L21"/>
+      <c r="M21"/>
+      <c r="N21"/>
+      <c r="O21"/>
+      <c r="P21"/>
+      <c r="Q21"/>
+      <c r="R21"/>
+      <c r="S21"/>
+      <c r="T21"/>
+      <c r="U21"/>
+      <c r="V21"/>
+      <c r="W21"/>
+      <c r="X21"/>
+      <c r="Y21"/>
+      <c r="Z21"/>
+      <c r="AA21"/>
+      <c r="AB21"/>
+      <c r="AC21"/>
+      <c r="AD21"/>
+      <c r="AE21"/>
+      <c r="AF21"/>
+      <c r="AG21"/>
+      <c r="AH21"/>
+      <c r="AI21"/>
+      <c r="AJ21"/>
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="G20:I20"/>
-    <mergeCell ref="G21:I21"/>
-    <mergeCell ref="G14:I14"/>
-    <mergeCell ref="G5:I5"/>
-    <mergeCell ref="G6:I6"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="G8:I8"/>
-    <mergeCell ref="G9:I9"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="G18:I18"/>
-    <mergeCell ref="G19:I19"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="G11:I11"/>
-    <mergeCell ref="G10:I10"/>
-    <mergeCell ref="G12:I12"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="G4:I4"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="D17:E17"/>
     <mergeCell ref="G15:I15"/>
     <mergeCell ref="G16:I16"/>
     <mergeCell ref="G17:I17"/>
     <mergeCell ref="D15:E15"/>
+    <mergeCell ref="G10:I10"/>
+    <mergeCell ref="G12:I12"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="G20:I20"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="G14:I14"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="G18:I18"/>
+    <mergeCell ref="G19:I19"/>
+    <mergeCell ref="G13:I13"/>
+    <mergeCell ref="D13:E13"/>
     <mergeCell ref="D14:E14"/>
-    <mergeCell ref="B1:I1"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="A2:I2"/>
-    <mergeCell ref="G3:I3"/>
-    <mergeCell ref="G4:I4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="G8:I8"/>
+    <mergeCell ref="G9:I9"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -4356,8 +4404,8 @@
   </sheetPr>
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4368,11 +4416,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="68" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
     </row>
     <row r="2" spans="1:3" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="75"/>
@@ -4380,13 +4428,13 @@
       <c r="C2" s="77"/>
     </row>
     <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A3" s="73" t="s">
+      <c r="A3" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="74" t="s">
-        <v>57</v>
-      </c>
-      <c r="C3" s="73" t="s">
+      <c r="B3" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="35" t="s">
         <v>24</v>
       </c>
     </row>
@@ -4395,10 +4443,10 @@
         <v>14</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -4406,10 +4454,10 @@
         <v>15</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -4417,10 +4465,10 @@
         <v>8</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -4428,10 +4476,10 @@
         <v>16</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="C7" s="28" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.2">
@@ -4439,21 +4487,21 @@
         <v>10</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="78" t="s">
+      <c r="A9" s="37" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="30" t="s">
-        <v>68</v>
-      </c>
-      <c r="C9" s="71" t="s">
-        <v>69</v>
+        <v>58</v>
+      </c>
+      <c r="C9" s="33" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4461,10 +4509,10 @@
         <v>12</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="C10" s="72" t="s">
-        <v>71</v>
+        <v>60</v>
+      </c>
+      <c r="C10" s="34" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>